<commit_message>
adjust lang code cz to cs and refactor language selector
</commit_message>
<xml_diff>
--- a/i18n/i18n.xlsx
+++ b/i18n/i18n.xlsx
@@ -61,7 +61,7 @@
     <t xml:space="preserve">PT</t>
   </si>
   <si>
-    <t xml:space="preserve">CZ</t>
+    <t xml:space="preserve">CS</t>
   </si>
   <si>
     <t xml:space="preserve">FI</t>
@@ -6271,11 +6271,11 @@
   <dimension ref="A1:Z90"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="C27" activeCellId="0" sqref="C27"/>
+      <selection pane="topRight" activeCell="M1" activeCellId="0" sqref="M1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>